<commit_message>
updated code in matrixporduct.cpp and updates excel measures
</commit_message>
<xml_diff>
--- a/assign1/doc/measures.xlsx
+++ b/assign1/doc/measures.xlsx
@@ -163,7 +163,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -194,6 +194,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -395,11 +399,11 @@
   </sheetPr>
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.67"/>
@@ -543,14 +547,14 @@
       <c r="G5" s="6" t="n">
         <v>600</v>
       </c>
-      <c r="H5" s="6" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>27095689</v>
-      </c>
-      <c r="J5" s="7" t="n">
-        <v>59844000</v>
+      <c r="H5" s="0" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="I5" s="8" t="n">
+        <v>27111997</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>57787192</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6" t="n">
@@ -559,16 +563,12 @@
       <c r="M5" s="6" t="n">
         <v>128</v>
       </c>
-      <c r="N5" s="6" t="n">
-        <v>89.68</v>
-      </c>
-      <c r="O5" s="6" t="n">
-        <v>70066740863</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>106487365376</v>
-      </c>
-      <c r="Q5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R5" s="6" t="n">
         <v>600</v>
       </c>
@@ -597,14 +597,14 @@
       <c r="G6" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="H6" s="6" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>125487563</v>
-      </c>
-      <c r="J6" s="7" t="n">
-        <v>278504989</v>
+      <c r="H6" s="0" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="I6" s="8" t="n">
+        <v>125734561</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>267747076</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6" t="n">
@@ -613,16 +613,12 @@
       <c r="M6" s="6" t="n">
         <v>256</v>
       </c>
-      <c r="N6" s="6" t="n">
-        <v>91.98</v>
-      </c>
-      <c r="O6" s="6" t="n">
-        <v>69629549486</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>115172195093</v>
-      </c>
-      <c r="Q6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R6" s="6" t="n">
         <v>1000</v>
       </c>
@@ -633,7 +629,7 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="n">
         <v>1400</v>
@@ -651,14 +647,14 @@
       <c r="G7" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="H7" s="6" t="n">
-        <v>2.54</v>
-      </c>
-      <c r="I7" s="7" t="n">
-        <v>344203100</v>
-      </c>
-      <c r="J7" s="7" t="n">
-        <v>756884728</v>
+      <c r="H7" s="0" t="n">
+        <v>1.583</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>346116682</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>708816444</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="n">
@@ -668,9 +664,11 @@
         <v>512</v>
       </c>
       <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R7" s="6" t="n">
         <v>1400</v>
       </c>
@@ -681,7 +679,7 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="n">
         <v>1800</v>
@@ -699,14 +697,14 @@
       <c r="G8" s="6" t="n">
         <v>1800</v>
       </c>
-      <c r="H8" s="6" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>731317297</v>
-      </c>
-      <c r="J8" s="7" t="n">
-        <v>1582469061</v>
+      <c r="H8" s="0" t="n">
+        <v>3.557</v>
+      </c>
+      <c r="I8" s="8" t="n">
+        <v>745271243</v>
+      </c>
+      <c r="J8" s="8" t="n">
+        <v>1439900904</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6" t="n">
@@ -716,9 +714,11 @@
         <v>128</v>
       </c>
       <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R8" s="6" t="n">
         <v>1800</v>
       </c>
@@ -729,7 +729,7 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="n">
         <v>2200</v>
@@ -747,14 +747,14 @@
       <c r="G9" s="6" t="n">
         <v>2200</v>
       </c>
-      <c r="H9" s="6" t="n">
-        <v>10.36</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>1334965239</v>
-      </c>
-      <c r="J9" s="7" t="n">
-        <v>2869607846</v>
+      <c r="H9" s="0" t="n">
+        <v>6.473</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>2073886158</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>2561167064</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6" t="n">
@@ -764,9 +764,11 @@
         <v>256</v>
       </c>
       <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R9" s="6" t="n">
         <v>2200</v>
       </c>
@@ -777,7 +779,7 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="n">
         <v>2600</v>
       </c>
@@ -794,14 +796,14 @@
       <c r="G10" s="6" t="n">
         <v>2600</v>
       </c>
-      <c r="H10" s="6" t="n">
-        <v>17.11</v>
-      </c>
-      <c r="I10" s="7" t="n">
-        <v>2203267700</v>
-      </c>
-      <c r="J10" s="7" t="n">
-        <v>4721863215</v>
+      <c r="H10" s="0" t="n">
+        <v>10.819</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>4412845122</v>
+      </c>
+      <c r="J10" s="8" t="n">
+        <v>4198690629</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6" t="n">
@@ -811,9 +813,11 @@
         <v>512</v>
       </c>
       <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R10" s="6" t="n">
         <v>2600</v>
       </c>
@@ -824,7 +828,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="n">
         <v>3000</v>
       </c>
@@ -841,14 +845,14 @@
       <c r="G11" s="6" t="n">
         <v>3000</v>
       </c>
-      <c r="H11" s="6" t="n">
-        <v>26.75</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <v>3384302638</v>
-      </c>
-      <c r="J11" s="7" t="n">
-        <v>7190187541</v>
+      <c r="H11" s="0" t="n">
+        <v>16.478</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>6780698787</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <v>6296071144</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6" t="n">
@@ -858,9 +862,11 @@
         <v>128</v>
       </c>
       <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R11" s="6" t="n">
         <v>3000</v>
       </c>
@@ -871,7 +877,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -880,14 +886,14 @@
       <c r="G12" s="6" t="n">
         <v>4096</v>
       </c>
-      <c r="H12" s="6" t="n">
-        <v>67.6</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>8637237294</v>
-      </c>
-      <c r="J12" s="7" t="n">
-        <v>18214065974</v>
+      <c r="H12" s="0" t="n">
+        <v>41.229</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>17553265709</v>
+      </c>
+      <c r="J12" s="8" t="n">
+        <v>16249690528</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="n">
@@ -897,9 +903,11 @@
         <v>256</v>
       </c>
       <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R12" s="6" t="n">
         <v>4096</v>
       </c>
@@ -910,7 +918,7 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -919,14 +927,14 @@
       <c r="G13" s="6" t="n">
         <v>6144</v>
       </c>
-      <c r="H13" s="6" t="n">
-        <v>227.04</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>29129375436</v>
-      </c>
-      <c r="J13" s="7" t="n">
-        <v>61368125691</v>
+      <c r="H13" s="0" t="n">
+        <v>139.299</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>59151207256</v>
+      </c>
+      <c r="J13" s="8" t="n">
+        <v>54420319247</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6" t="n">
@@ -936,9 +944,11 @@
         <v>512</v>
       </c>
       <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R13" s="6" t="n">
         <v>6144</v>
       </c>
@@ -949,7 +959,7 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
@@ -960,15 +970,9 @@
       <c r="G14" s="6" t="n">
         <v>8192</v>
       </c>
-      <c r="H14" s="6" t="n">
-        <v>537.18</v>
-      </c>
-      <c r="I14" s="7" t="n">
-        <v>69001196060</v>
-      </c>
-      <c r="J14" s="7" t="n">
-        <v>145261351152</v>
-      </c>
+      <c r="H14" s="0"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6" t="n">
         <v>10240</v>
@@ -977,9 +981,11 @@
         <v>128</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R14" s="6" t="n">
         <v>8192</v>
       </c>
@@ -990,7 +996,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1003,15 +1009,9 @@
       <c r="G15" s="6" t="n">
         <v>10240</v>
       </c>
-      <c r="H15" s="6" t="n">
-        <v>1074.36</v>
-      </c>
-      <c r="I15" s="7" t="n">
-        <v>138002392120</v>
-      </c>
-      <c r="J15" s="7" t="n">
-        <v>290522702304</v>
-      </c>
+      <c r="H15" s="0"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6" t="n">
         <v>10240</v>
@@ -1020,9 +1020,11 @@
         <v>256</v>
       </c>
       <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R15" s="6" t="n">
         <v>10240</v>
       </c>
@@ -1053,9 +1055,11 @@
         <v>512</v>
       </c>
       <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
@@ -1198,7 +1202,7 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="n">
         <v>2600</v>
       </c>
@@ -1213,19 +1217,10 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="6" t="n">
-        <f aca="false">AVERAGE(M21:O21)</f>
-        <v>91.9793333333333</v>
-      </c>
-      <c r="M21" s="6" t="n">
-        <v>89.691</v>
-      </c>
-      <c r="N21" s="6" t="n">
-        <v>98.783</v>
-      </c>
-      <c r="O21" s="6" t="n">
-        <v>87.464</v>
-      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6" t="n">
@@ -1238,7 +1233,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="n">
         <v>3000</v>
       </c>
@@ -1253,19 +1248,10 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="6" t="n">
-        <f aca="false">AVERAGE(M22:O22)</f>
-        <v>69629549486.3333</v>
-      </c>
-      <c r="M22" s="7" t="n">
-        <v>69488621365</v>
-      </c>
-      <c r="N22" s="7" t="n">
-        <v>69886426393</v>
-      </c>
-      <c r="O22" s="7" t="n">
-        <v>69513600701</v>
-      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6" t="n">
@@ -1278,7 +1264,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1291,19 +1277,10 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="6" t="n">
-        <f aca="false">AVERAGE(M23:O23)</f>
-        <v>115172195093</v>
-      </c>
-      <c r="M23" s="7" t="n">
-        <v>101954945509</v>
-      </c>
-      <c r="N23" s="7" t="n">
-        <v>111788148004</v>
-      </c>
-      <c r="O23" s="7" t="n">
-        <v>131773491766</v>
-      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6" t="n">
@@ -1458,7 +1435,7 @@
       <c r="X28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="8"/>
+      <c r="B29" s="9"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -1506,7 +1483,7 @@
       <c r="X30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="9"/>
+      <c r="B31" s="10"/>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>

</xml_diff>